<commit_message>
new zoop energy data added and functions made
</commit_message>
<xml_diff>
--- a/data/zoop_energy_data/Energy_Density_Data.xlsx
+++ b/data/zoop_energy_data/Energy_Density_Data.xlsx
@@ -5,23 +5,22 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pndph\Documents\Classes and Working Groups\NCEAS\Git_Hub_Repo\data\PD_zoo_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pndph\Documents\Classes and Working Groups\NCEAS\Work_Repo\data\zoop_energy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6449AD-35EB-4F51-BBD0-E18780C9E80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12010BA-A122-41A0-B216-99C8BF7E6C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="5890" windowWidth="16570" windowHeight="7480" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4040" yWindow="1100" windowWidth="16570" windowHeight="9670" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="zoo_energy_catagories" sheetId="6" r:id="rId1"/>
-    <sheet name="zoo_energy_groups" sheetId="7" r:id="rId2"/>
-    <sheet name="zoo_energy_dry" sheetId="1" r:id="rId3"/>
-    <sheet name="zoo_energy_wet" sheetId="5" r:id="rId4"/>
-    <sheet name="zoo_energy_digestibility" sheetId="4" r:id="rId5"/>
-    <sheet name="zoo_energy_ratio" sheetId="3" r:id="rId6"/>
+    <sheet name="zoo_energy_groups" sheetId="7" r:id="rId1"/>
+    <sheet name="zoo_energy_dry" sheetId="1" r:id="rId2"/>
+    <sheet name="zoo_energy_wet" sheetId="5" r:id="rId3"/>
+    <sheet name="zoo_energy_digestibility" sheetId="4" r:id="rId4"/>
+    <sheet name="zoo_energy_ratio" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">zoo_energy_dry!$A$1:$A$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">zoo_energy_dry!$A$1:$A$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="69">
   <si>
     <t>Cladoceran</t>
   </si>
@@ -53,15 +52,6 @@
     <t>Amphipods</t>
   </si>
   <si>
-    <t>Herbivorous Calanoid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Predatory Calanoid </t>
-  </si>
-  <si>
-    <t>Cyclopoid</t>
-  </si>
-  <si>
     <t>Rotifers</t>
   </si>
   <si>
@@ -95,12 +85,6 @@
     <t>energy_density_j_per_g_dry_mass</t>
   </si>
   <si>
-    <t>Copepoda</t>
-  </si>
-  <si>
-    <t>subclass</t>
-  </si>
-  <si>
     <t>Hanson 1997</t>
   </si>
   <si>
@@ -125,9 +109,6 @@
     <t>secondary</t>
   </si>
   <si>
-    <t>Foy 1999</t>
-  </si>
-  <si>
     <t>dry_to_wet_ratio</t>
   </si>
   <si>
@@ -146,9 +127,6 @@
     <t>tigriopus californicus</t>
   </si>
   <si>
-    <t>catanus helgolandicus</t>
-  </si>
-  <si>
     <t>calanus finmarchicus</t>
   </si>
   <si>
@@ -161,9 +139,6 @@
     <t>diaptomus siciloides</t>
   </si>
   <si>
-    <t xml:space="preserve">Omnivorous Calanoid </t>
-  </si>
-  <si>
     <t>diaptomus leptopus</t>
   </si>
   <si>
@@ -179,9 +154,6 @@
     <t>Vijverberg 1976</t>
   </si>
   <si>
-    <t>Calanoid</t>
-  </si>
-  <si>
     <t>Diaptomus hyalinus</t>
   </si>
   <si>
@@ -194,9 +166,6 @@
     <t>Euphonia affinis</t>
   </si>
   <si>
-    <t>sub_group</t>
-  </si>
-  <si>
     <t>Tupltromvsis bowmani</t>
   </si>
   <si>
@@ -234,6 +203,51 @@
   </si>
   <si>
     <t>Pauli 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predatory Copepoda </t>
+  </si>
+  <si>
+    <t>Herbivorous Copepoda</t>
+  </si>
+  <si>
+    <t>asplanchna brightwellii</t>
+  </si>
+  <si>
+    <t>Dumont 1975</t>
+  </si>
+  <si>
+    <t>Cyclopoida</t>
+  </si>
+  <si>
+    <t>Limnocalanus johanseni</t>
+  </si>
+  <si>
+    <t>Comita 1956</t>
+  </si>
+  <si>
+    <t>Diaptomus minutus</t>
+  </si>
+  <si>
+    <t>Cyclops bicuspidatus thomasi</t>
+  </si>
+  <si>
+    <t>Holopedium gibberum</t>
+  </si>
+  <si>
+    <t>Bosmina longirostris</t>
+  </si>
+  <si>
+    <t>Kellicottia sp.</t>
+  </si>
+  <si>
+    <t>Daphnia dubia</t>
+  </si>
+  <si>
+    <t>Schindler 1971</t>
+  </si>
+  <si>
+    <t>calanus helgolandicus</t>
   </si>
 </sst>
 </file>
@@ -564,82 +578,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{591EA514-A6A7-41B2-AB07-2ED56ADD8291}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4AD6A0-BF1A-4D70-B355-9C73B407CDB8}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -647,67 +632,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4AD6A0-BF1A-4D70-B355-9C73B407CDB8}">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
@@ -717,22 +652,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -743,17 +678,17 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <f>(2972+4312)/0.16/2</f>
         <v>22762.5</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -761,19 +696,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>17200</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -781,19 +716,19 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>20400</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -804,76 +739,76 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>22843</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>23718</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6">
-        <v>21765.5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>17045</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7">
-        <v>23718</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>2</v>
+      <c r="B8" t="s">
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E8">
-        <v>17045</v>
+        <v>21681.488000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -881,19 +816,19 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E9">
-        <v>21681.488000000001</v>
+        <v>16966.62</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -901,19 +836,19 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E10">
-        <v>16966.62</v>
+        <v>17238.32</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -921,396 +856,398 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E11">
-        <v>17238.32</v>
+        <v>21213.5</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>0</v>
+      <c r="A12" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E12">
-        <v>21213.5</v>
+        <v>23219.899999999998</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>17</v>
+      <c r="A13" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E13">
-        <v>23219.899999999998</v>
+        <v>22572</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>17</v>
+      <c r="A14" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E14">
-        <v>22572</v>
+        <v>24720.519999999997</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E15">
-        <v>24720.519999999997</v>
+        <v>31065.759999999998</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E16">
-        <v>31065.759999999998</v>
+        <v>30848.399999999998</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E17">
-        <v>30848.399999999998</v>
+        <v>22856.239999999998</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E18">
-        <v>22856.239999999998</v>
+        <v>23098.679999999997</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E19">
-        <v>23098.679999999997</v>
+        <v>22296.12</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E20">
-        <v>22296.12</v>
+        <v>23587.739999999998</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E21">
-        <v>23587.739999999998</v>
+        <v>22555.279999999999</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E22">
-        <v>22555.279999999999</v>
+        <v>22722.48</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E23">
-        <v>22722.48</v>
+        <v>22898.039999999997</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>5</v>
+      <c r="A24" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E24">
-        <v>22898.039999999997</v>
+        <v>26242.039999999997</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>5</v>
+      <c r="A25" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E25">
-        <v>24925.339999999997</v>
+        <v>26363.26</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E26">
-        <v>26242.039999999997</v>
+        <v>25581.599999999999</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>3</v>
+      <c r="A27" t="s">
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E27">
-        <v>26363.26</v>
+        <v>24440.46</v>
       </c>
       <c r="F27" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E28">
-        <v>25581.599999999999</v>
+        <v>26555.539999999997</v>
       </c>
       <c r="F28" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>0</v>
+      <c r="A29" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E29">
-        <v>24440.46</v>
+        <f>4426.3*4.18</f>
+        <v>18501.934000000001</v>
       </c>
       <c r="F29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E30">
-        <v>26555.539999999997</v>
+        <f>4.4*1000*4.18</f>
+        <v>18392</v>
       </c>
       <c r="F30" t="s">
         <v>44</v>
@@ -1318,222 +1255,228 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E31">
-        <f>4426.3*4.18</f>
-        <v>18501.934000000001</v>
+        <f>4.71*1000*4.18</f>
+        <v>19687.8</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E32">
-        <f>4.4*1000*4.18</f>
-        <v>18392</v>
+        <v>26018</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>6</v>
+      <c r="A33" t="s">
+        <v>0</v>
       </c>
       <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33">
+        <v>19869.629999999997</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33">
-        <f>4.71*1000*4.18</f>
-        <v>19687.8</v>
-      </c>
-      <c r="F33" t="s">
-        <v>56</v>
-      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34">
+        <v>26781</v>
+      </c>
+      <c r="F34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35">
+        <v>19927.453333333335</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36">
+        <v>19813.199999999997</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37">
+        <v>20337.789999999997</v>
+      </c>
+      <c r="F37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A30" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B33:F37">
+    <sortCondition ref="B33:B37"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA17065-39FE-4264-88CB-BEB24B611442}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.6328125" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E2">
-        <v>4410</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3">
-        <v>2930</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4">
-        <v>2090</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5">
-        <v>3600</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6">
         <f>810*4.18</f>
         <v>3385.7999999999997</v>
       </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1541,13 +1484,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAE9FAC-7F47-482E-9162-E07DA05FFE29}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1562,22 +1505,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1585,19 +1528,19 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>0.627</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1605,19 +1548,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>0.80900000000000005</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1626,18 +1569,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EFD9D4-4ECD-467B-85BC-BACF641DC1E9}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A8:XFD9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.26953125" customWidth="1"/>
@@ -1647,22 +1590,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1673,16 +1616,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>0.16</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1693,216 +1636,256 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>0.11</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>0.04</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4">
-        <v>0.125</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>0.26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
         <v>0.04</v>
       </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6">
-        <v>0.26</v>
-      </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E7">
-        <v>0.04</v>
+        <v>0.151</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E8">
-        <v>0.151</v>
+        <v>0.10050000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E9">
-        <v>0.10050000000000001</v>
+        <v>3.95E-2</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E10">
-        <v>3.95E-2</v>
+        <v>0.11550000000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E11">
-        <v>0.11550000000000001</v>
+        <v>4.4500000000000005E-2</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E12">
-        <v>4.4500000000000005E-2</v>
+        <v>4.9500000000000002E-2</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E13">
-        <v>4.9500000000000002E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14">
+        <v>0.115</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15">
+        <v>0.09</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more zoop energy density data
</commit_message>
<xml_diff>
--- a/data/zoop_energy_data/Energy_Density_Data.xlsx
+++ b/data/zoop_energy_data/Energy_Density_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pndph\Documents\Classes and Working Groups\NCEAS\Work_Repo\data\zoop_energy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12010BA-A122-41A0-B216-99C8BF7E6C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73206B59-3C0C-408F-B4E9-04D6FCB6FC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="1100" windowWidth="16570" windowHeight="9670" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9770" yWindow="850" windowWidth="16570" windowHeight="9670" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zoo_energy_groups" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="77">
   <si>
     <t>Cladoceran</t>
   </si>
@@ -248,6 +248,30 @@
   </si>
   <si>
     <t>calanus helgolandicus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themisto pacifica </t>
+  </si>
+  <si>
+    <t>T. japonica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primno abyssalis </t>
+  </si>
+  <si>
+    <t>Cyphocaris challengeri</t>
+  </si>
+  <si>
+    <t>Yamada 2003</t>
+  </si>
+  <si>
+    <t>Yamada 2004</t>
+  </si>
+  <si>
+    <t>Yamada 2005</t>
+  </si>
+  <si>
+    <t>Yamada 2006</t>
   </si>
 </sst>
 </file>
@@ -1572,10 +1596,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EFD9D4-4ECD-467B-85BC-BACF641DC1E9}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1888,6 +1912,86 @@
         <v>60</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16">
+        <v>0.22799999999999998</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17">
+        <v>0.22299999999999998</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18">
+        <v>0.22599999999999998</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19">
+        <v>0.19899999999999995</v>
+      </c>
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more zoop energy data added and code testing diagrams
</commit_message>
<xml_diff>
--- a/data/zoop_energy_data/Energy_Density_Data.xlsx
+++ b/data/zoop_energy_data/Energy_Density_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pndph\Documents\Classes and Working Groups\NCEAS\Work_Repo\data\zoop_energy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73206B59-3C0C-408F-B4E9-04D6FCB6FC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3626253-A891-4B57-B8EB-D45665D87635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9770" yWindow="850" windowWidth="16570" windowHeight="9670" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zoo_energy_groups" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="88">
   <si>
     <t>Cladoceran</t>
   </si>
@@ -272,6 +272,39 @@
   </si>
   <si>
     <t>Yamada 2006</t>
+  </si>
+  <si>
+    <t>Calanus cristatus</t>
+  </si>
+  <si>
+    <t>Calanus plumchrus</t>
+  </si>
+  <si>
+    <t>Calanus pacificus</t>
+  </si>
+  <si>
+    <t>Eucalanus bungii</t>
+  </si>
+  <si>
+    <t>Candacia columbiae</t>
+  </si>
+  <si>
+    <t>Pontellina plumata</t>
+  </si>
+  <si>
+    <t>Metridia okhotensis</t>
+  </si>
+  <si>
+    <t>omori 1969</t>
+  </si>
+  <si>
+    <t>Paraeuchaeta birostrata</t>
+  </si>
+  <si>
+    <t>Disseta palumboi</t>
+  </si>
+  <si>
+    <t>Candacia ethiopica</t>
   </si>
 </sst>
 </file>
@@ -320,9 +353,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +694,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1596,10 +1630,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EFD9D4-4ECD-467B-85BC-BACF641DC1E9}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1992,6 +2026,207 @@
         <v>76</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20">
+        <v>0.22</v>
+      </c>
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21">
+        <v>0.27699999999999997</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22">
+        <f>(0.197+0.212)/2</f>
+        <v>0.20450000000000002</v>
+      </c>
+      <c r="F22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23">
+        <v>0.12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24">
+        <v>0.185</v>
+      </c>
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25">
+        <v>0.188</v>
+      </c>
+      <c r="F25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27">
+        <v>0.14300000000000002</v>
+      </c>
+      <c r="F27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="F28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="F29" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FMWT regional averaging added to FWMT analysis code
</commit_message>
<xml_diff>
--- a/data/zoop_energy_data/Energy_Density_Data.xlsx
+++ b/data/zoop_energy_data/Energy_Density_Data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pndph\Documents\Classes and Working Groups\NCEAS\Work_Repo\data\zoop_energy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3626253-A891-4B57-B8EB-D45665D87635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D590FB-2DC5-4C56-ADE2-AB0C41A32EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11265" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zoo_energy_groups" sheetId="7" r:id="rId1"/>
     <sheet name="zoo_energy_dry" sheetId="1" r:id="rId2"/>
-    <sheet name="zoo_energy_wet" sheetId="5" r:id="rId3"/>
-    <sheet name="zoo_energy_digestibility" sheetId="4" r:id="rId4"/>
-    <sheet name="zoo_energy_ratio" sheetId="3" r:id="rId5"/>
+    <sheet name="feeding_cite" sheetId="8" r:id="rId3"/>
+    <sheet name="zoo_energy_wet" sheetId="5" r:id="rId4"/>
+    <sheet name="zoo_energy_digestibility" sheetId="4" r:id="rId5"/>
+    <sheet name="zoo_energy_ratio" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">zoo_energy_dry!$A$1:$A$28</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="103">
   <si>
     <t>Cladoceran</t>
   </si>
@@ -305,13 +306,70 @@
   </si>
   <si>
     <t>Candacia ethiopica</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>Conover</t>
+  </si>
+  <si>
+    <t>The Feeding Behavior and Respiration of Some Marine Planktonic Crustacea</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <r>
+      <t>Grazing and ingestion rates of nauplii, copepodids and adults of the marine planktonic copepod </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>Calanus helgolandicus</t>
+    </r>
+  </si>
+  <si>
+    <t>Paffenhofer</t>
+  </si>
+  <si>
+    <t>BEHAVIORAL AND MORPHOLOGICAL INFLUENCES ON PREDATORY INTERACTIONS AMONG MARINE COPEPODS</t>
+  </si>
+  <si>
+    <t>landray</t>
+  </si>
+  <si>
+    <t>Overwintering strategies of the calanoid copepod Calanus plumchrus in a periodically anoxic British Columbia fjord</t>
+  </si>
+  <si>
+    <t>Cowen</t>
+  </si>
+  <si>
+    <t>Several sources of wikipedia page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +389,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Georgia"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -643,45 +708,45 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
   </sheetData>
@@ -694,21 +759,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6328125" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -728,7 +793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -749,7 +814,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -769,7 +834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -789,7 +854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -809,7 +874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -829,7 +894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -849,7 +914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -869,7 +934,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -889,7 +954,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -909,7 +974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -929,7 +994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -949,7 +1014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -969,7 +1034,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -989,7 +1054,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1009,7 +1074,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
@@ -1029,7 +1094,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -1049,7 +1114,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -1069,7 +1134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -1089,7 +1154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -1109,7 +1174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -1129,7 +1194,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -1149,7 +1214,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
@@ -1169,7 +1234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -1189,7 +1254,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -1209,7 +1274,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -1229,7 +1294,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1314,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
@@ -1269,7 +1334,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -1290,7 +1355,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -1311,7 +1376,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -1332,7 +1397,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
@@ -1352,7 +1417,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1437,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
@@ -1392,7 +1457,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1412,7 +1477,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +1497,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -1452,10 +1517,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
   </sheetData>
@@ -1469,6 +1534,178 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDB5B2D-52B0-402D-963A-873F6F15E85B}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2">
+        <v>1971</v>
+      </c>
+      <c r="F2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3">
+        <v>1960</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4">
+        <v>1960</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5">
+        <v>1960</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6">
+        <v>1988</v>
+      </c>
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7">
+        <v>1982</v>
+      </c>
+      <c r="F7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA17065-39FE-4264-88CB-BEB24B611442}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F4"/>
@@ -1477,17 +1714,17 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6328125" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1507,7 +1744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1528,11 +1765,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
@@ -1542,7 +1779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAE9FAC-7F47-482E-9162-E07DA05FFE29}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F3"/>
@@ -1551,17 +1788,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1581,7 +1818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1601,7 +1838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1627,26 +1864,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EFD9D4-4ECD-467B-85BC-BACF641DC1E9}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.26953125" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1666,7 +1903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1686,7 +1923,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1706,7 +1943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1746,7 +1983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1766,7 +2003,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1786,7 +2023,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1806,7 +2043,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1826,7 +2063,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +2083,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1866,7 +2103,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1886,7 +2123,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1906,7 +2143,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -1926,7 +2163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1946,7 +2183,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1966,7 +2203,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1986,7 +2223,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2006,7 +2243,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2026,7 +2263,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -2046,7 +2283,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
@@ -2066,7 +2303,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
@@ -2087,7 +2324,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -2107,7 +2344,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -2127,7 +2364,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -2147,7 +2384,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -2167,7 +2404,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
@@ -2187,7 +2424,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -2207,7 +2444,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
just changed the zoop energy script to save image
</commit_message>
<xml_diff>
--- a/data/zoop_energy_data/Energy_Density_Data.xlsx
+++ b/data/zoop_energy_data/Energy_Density_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pndph\Documents\Classes and Working Groups\NCEAS\Work_Repo\data\zoop_energy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7B8580-924B-46D4-8E11-9683A6A5DD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C24ADE-B689-4221-B303-1324B2029BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31305" yWindow="2505" windowWidth="21600" windowHeight="11265" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zoo_energy_groups" sheetId="7" r:id="rId1"/>
@@ -984,7 +984,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,25 +1045,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F3">
-        <v>17200</v>
+        <v>26363.26</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1091,59 +1091,61 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F5">
-        <v>22843</v>
+        <f>4.4*1000*4.18</f>
+        <v>18392</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>16966.62</v>
+        <f>4.71*1000*4.18</f>
+        <v>19687.8</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -1152,7 +1154,7 @@
         <v>21</v>
       </c>
       <c r="F7">
-        <v>17238.32</v>
+        <v>24720.519999999997</v>
       </c>
       <c r="G7" t="s">
         <v>25</v>
@@ -1160,13 +1162,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -1175,7 +1177,7 @@
         <v>21</v>
       </c>
       <c r="F8">
-        <v>21213.5</v>
+        <v>30848.399999999998</v>
       </c>
       <c r="G8" t="s">
         <v>25</v>
@@ -1183,59 +1185,59 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F9">
-        <v>19927.453333333335</v>
+        <v>22572</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
       <c r="F10">
-        <v>20400</v>
+        <v>31065.759999999998</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -1244,30 +1246,30 @@
         <v>35</v>
       </c>
       <c r="F11">
-        <v>19813.199999999997</v>
+        <v>25581.599999999999</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
       </c>
       <c r="F12">
-        <v>23718</v>
+        <v>22843</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
@@ -1275,82 +1277,82 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F13">
-        <v>21681.488000000001</v>
+        <v>26781</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F14">
-        <v>24440.46</v>
+        <v>16966.62</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F15">
-        <v>26363.26</v>
+        <v>17238.32</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
@@ -1359,7 +1361,7 @@
         <v>21</v>
       </c>
       <c r="F16">
-        <v>24720.519999999997</v>
+        <v>21213.5</v>
       </c>
       <c r="G16" t="s">
         <v>25</v>
@@ -1367,59 +1369,59 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
         <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F17">
-        <v>30848.399999999998</v>
+        <v>19927.453333333335</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
       <c r="F18">
-        <v>22572</v>
+        <v>20400</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
@@ -1428,7 +1430,7 @@
         <v>21</v>
       </c>
       <c r="F19">
-        <v>31065.759999999998</v>
+        <v>22856.239999999998</v>
       </c>
       <c r="G19" t="s">
         <v>25</v>
@@ -1436,36 +1438,36 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F20">
-        <v>25581.599999999999</v>
+        <v>23098.679999999997</v>
       </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
         <v>24</v>
@@ -1474,38 +1476,38 @@
         <v>35</v>
       </c>
       <c r="F21">
-        <v>26781</v>
+        <v>26242.039999999997</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F22">
-        <v>26242.039999999997</v>
+        <v>22555.279999999999</v>
       </c>
       <c r="G22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>52</v>
@@ -1520,7 +1522,7 @@
         <v>21</v>
       </c>
       <c r="F23">
-        <v>22555.279999999999</v>
+        <v>22722.48</v>
       </c>
       <c r="G23" t="s">
         <v>25</v>
@@ -1528,53 +1530,53 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F24">
-        <v>22722.48</v>
+        <v>26018</v>
       </c>
       <c r="G24" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F25">
-        <v>26018</v>
+        <v>22296.12</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>52</v>
@@ -1589,7 +1591,7 @@
         <v>21</v>
       </c>
       <c r="F26">
-        <v>22296.12</v>
+        <v>23587.739999999998</v>
       </c>
       <c r="G26" t="s">
         <v>25</v>
@@ -1597,130 +1599,128 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
         <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F27">
-        <v>23587.739999999998</v>
+        <v>26555.539999999997</v>
       </c>
       <c r="G27" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F28">
-        <v>26555.539999999997</v>
+        <v>17200</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
         <v>24</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F29">
-        <v>23219.899999999998</v>
+        <v>19813.199999999997</v>
       </c>
       <c r="G29" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F30">
-        <f>(2972+4312)/0.16/2</f>
-        <v>22762.5</v>
+        <v>20337.789999999997</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F31">
-        <f>4426.3*4.18</f>
-        <v>18501.934000000001</v>
+        <v>23718</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D32" t="s">
         <v>24</v>
@@ -1729,7 +1729,7 @@
         <v>21</v>
       </c>
       <c r="F32">
-        <v>22856.239999999998</v>
+        <v>21681.488000000001</v>
       </c>
       <c r="G32" t="s">
         <v>25</v>
@@ -1737,25 +1737,25 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>51</v>
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
         <v>24</v>
       </c>
       <c r="E33" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F33">
-        <v>23098.679999999997</v>
+        <v>24440.46</v>
       </c>
       <c r="G33" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1783,37 +1783,37 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F35">
-        <f>4.4*1000*4.18</f>
-        <v>18392</v>
+        <f>(2972+4312)/0.16/2</f>
+        <v>22762.5</v>
       </c>
       <c r="G35" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>141</v>
       </c>
       <c r="D36" t="s">
         <v>24</v>
@@ -1822,34 +1822,34 @@
         <v>35</v>
       </c>
       <c r="F36">
-        <f>4.71*1000*4.18</f>
-        <v>19687.8</v>
+        <f>4426.3*4.18</f>
+        <v>18501.934000000001</v>
       </c>
       <c r="G36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E37" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F37">
-        <v>20337.789999999997</v>
+        <v>23219.899999999998</v>
       </c>
       <c r="G37" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1859,8 +1859,8 @@
       <c r="B41" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G41">
-    <sortCondition ref="B2:B41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G37">
+    <sortCondition ref="C2:C37"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2045,7 +2045,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2204,7 +2204,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:B22"/>
     </sheetView>
   </sheetViews>
@@ -2215,7 +2215,7 @@
     <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.28515625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2810,7 +2810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72932407-8C53-4F63-9471-927903B31268}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -3227,8 +3227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019D8B8A-3984-4937-96A7-56732934F7F2}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>